<commit_message>
modified to latest version
</commit_message>
<xml_diff>
--- a/EickhoffALE/contrasts/painHealthyAnalyses_20190401.xlsx
+++ b/EickhoffALE/contrasts/painHealthyAnalyses_20190401.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10440" yWindow="460" windowWidth="19220" windowHeight="20540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19220" windowHeight="20540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -62,9 +62,6 @@
     <t>+activation</t>
   </si>
   <si>
-    <t>painHealthyCoords_20190401.mat</t>
-  </si>
-  <si>
     <t>+activationpainBaseline</t>
   </si>
   <si>
@@ -144,6 +141,9 @@
   </si>
   <si>
     <t>thermal</t>
+  </si>
+  <si>
+    <t>painHealthyCoords_20190426.mat</t>
   </si>
 </sst>
 </file>
@@ -482,7 +482,7 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -498,10 +498,10 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -515,16 +515,16 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -532,10 +532,10 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>1</v>
@@ -549,10 +549,10 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>1</v>
@@ -566,10 +566,10 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>1</v>
@@ -580,10 +580,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>1</v>
@@ -597,16 +597,16 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -614,16 +614,16 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -631,30 +631,30 @@
         <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -662,16 +662,16 @@
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -679,10 +679,10 @@
         <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>1</v>
@@ -702,10 +702,10 @@
         <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>1</v>
@@ -725,10 +725,10 @@
         <v>0</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>1</v>
@@ -745,10 +745,10 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>1</v>
@@ -768,16 +768,16 @@
         <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -785,16 +785,16 @@
         <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -802,30 +802,30 @@
         <v>0</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -833,16 +833,16 @@
         <v>4</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F20" s="5"/>
     </row>
@@ -851,19 +851,19 @@
         <v>4</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -871,34 +871,34 @@
         <v>0</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F22" s="5"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B23" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -906,16 +906,16 @@
         <v>4</v>
       </c>
       <c r="B24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -923,16 +923,16 @@
         <v>4</v>
       </c>
       <c r="B25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -940,30 +940,30 @@
         <v>0</v>
       </c>
       <c r="B26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -971,16 +971,16 @@
         <v>4</v>
       </c>
       <c r="B28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C28" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>